<commit_message>
changed homepage hero font
</commit_message>
<xml_diff>
--- a/info/Stage Fright Project Plan.xlsx
+++ b/info/Stage Fright Project Plan.xlsx
@@ -5,11 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps25skalb\Documents\test-deploy\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps25skalb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F98EB31-B337-474C-A3C4-4F3622937DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="RvfQihVZtCromHE+XU/UDsTkhKhCDY5ZSnNO0L7utEjwuXx77IT/X4IfwalRO0EpQeNy+hXtGjXFmab2sRVEtg==" workbookSaltValue="OxriCbgZHpNSsIAzpt603Q==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D780763-0AB3-44F0-8F91-3FB713A9A46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="4170" windowWidth="40260" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Create Logo, albums, songs and merch</t>
   </si>
@@ -233,13 +232,16 @@
   </si>
   <si>
     <t>New Menu</t>
+  </si>
+  <si>
+    <t>Fix Navbar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,12 +311,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -665,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -723,7 +719,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1141,7 +1136,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1387,7 +1382,7 @@
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="42"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1425,7 +1420,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="13"/>
@@ -1453,12 +1448,12 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kWjRMJuZ5hx6xY7RrpO/W7G0tbrbJ6TcfntpW89AWiktTRjX2J8IWb3CfprWzFV3C0aFJomX+byB5Vcsw5lSKQ==" saltValue="2F5aR7wh0iJPNv5sNhmikw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="tjZktos/tqwqzmFVtiUT9E0ZRH5IlbsCbcQcarJSCo8GaTF+3st4qoW68oz80FfSrseBosRXVc2qqJxS/2vMdw==" saltValue="7e8ArAkUS1u3zvTCEvzCkw==" spinCount="100000" sqref="A25 B2:J19" name="Im Jaking it"/>
   </protectedRanges>
@@ -1475,7 +1470,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2063,15 +2058,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5580F25D-1F12-491F-81BA-04B8517773EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bf135858-4173-4f00-afdf-ebb7dec0ff81"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bf135858-4173-4f00-afdf-ebb7dec0ff81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>